<commit_message>
Modified Test Data sheet
</commit_message>
<xml_diff>
--- a/ServiceNowQAAutomation/SNOWQA/testdata/Change_Management_TestData.xlsx
+++ b/ServiceNowQAAutomation/SNOWQA/testdata/Change_Management_TestData.xlsx
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="28">
   <si>
     <t>Serial No.</t>
   </si>
@@ -126,44 +126,16 @@
     <t>Failed</t>
   </si>
   <si>
-    <t>CHG0037345</t>
-  </si>
-  <si>
-    <t>2017-08-25 15:36:30</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>CHG0037347</t>
-  </si>
-  <si>
-    <t>CHG0037350</t>
-  </si>
-  <si>
-    <t>CHG0037354</t>
-  </si>
-  <si>
-    <t>CHG0037355</t>
-  </si>
-  <si>
-    <t>CHG0037356</t>
-  </si>
-  <si>
-    <t>CHG0037357</t>
-  </si>
-  <si>
-    <t>CHG0037359</t>
-  </si>
-  <si>
     <t>CHG0037360</t>
+  </si>
+  <si>
+    <t>2017-09-01 15:36:30</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -576,19 +548,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="8.7109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="22.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="32.28515625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="16.5703125" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="31.42578125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="8.5703125" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="22.140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="32.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="16" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="31.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="18.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
@@ -652,7 +624,7 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" t="s">

</xml_diff>

<commit_message>
Changes made on below files ChangeReusables ChangePage.java Constants.properties SnowReporter.java DropDowns.java Capabilities.properties
</commit_message>
<xml_diff>
--- a/ServiceNowQAAutomation/SNOWQA/testdata/Change_Management_TestData.xlsx
+++ b/ServiceNowQAAutomation/SNOWQA/testdata/Change_Management_TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="45" windowWidth="15150" windowHeight="7995"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="13290" windowHeight="4800"/>
   </bookViews>
   <sheets>
     <sheet name="Smoke_Suite" sheetId="3" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="33">
   <si>
     <t>Serial No.</t>
   </si>
@@ -123,19 +123,35 @@
     <t>Requested End Date</t>
   </si>
   <si>
-    <t>Failed</t>
-  </si>
-  <si>
-    <t>CHG0037360</t>
-  </si>
-  <si>
     <t>2017-09-01 15:36:30</t>
+  </si>
+  <si>
+    <t>Passed</t>
+  </si>
+  <si>
+    <t>CHG0030030</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>CHG0037650</t>
+  </si>
+  <si>
+    <t>CHG0037652</t>
+  </si>
+  <si>
+    <t>CHG0037653</t>
+  </si>
+  <si>
+    <t>CHG0037654</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -542,25 +558,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="22.140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="32.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="31.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="18.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="8.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="22.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="32.28515625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="16.5703125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="31.42578125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="8.5703125" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="18.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
@@ -624,11 +640,11 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F2" s="6" t="s">
         <v>8</v>
@@ -658,7 +674,7 @@
         <v>21</v>
       </c>
       <c r="O2" s="9" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="P2" s="3"/>
       <c r="Q2" s="3"/>
@@ -670,7 +686,9 @@
       <c r="B3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="3"/>
+      <c r="C3" t="s">
+        <v>26</v>
+      </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="6" t="s">
@@ -711,9 +729,13 @@
       <c r="B4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="3"/>
+      <c r="C4" t="s">
+        <v>32</v>
+      </c>
       <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
+      <c r="E4" t="s">
+        <v>26</v>
+      </c>
       <c r="F4" s="6" t="s">
         <v>8</v>
       </c>

</xml_diff>